<commit_message>
study 3 done for #146
</commit_message>
<xml_diff>
--- a/resources_studies/Cotton2014/gene_locations_cotton14_dup.xlsx
+++ b/resources_studies/Cotton2014/gene_locations_cotton14_dup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karinemoussa/Documents/DrLiu_Lab/Shiny_Apps/xci-app-1/resources_studies/Cotton2014/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6782A3-8F2E-5746-8EE9-9E4ADBEBC1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9A3576-2078-EA43-94EA-6BBD2BB3B106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="24980" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="920" yWindow="680" windowWidth="24980" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -536,7 +536,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>